<commit_message>
New branch due to synching problems
</commit_message>
<xml_diff>
--- a/Permittivities-permeabilities-conductivities.xlsx
+++ b/Permittivities-permeabilities-conductivities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6296818d0b3f89ce/Universiteit/MA1EE/Semester 2/Communication channels/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\OneDrive\Universiteit\MA1EE\Semester 2\Communication channels\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="36" documentId="8_{DE20D204-14EF-4C81-A722-C94FCADEF3C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{9CC13422-334B-4CC3-9D12-A3F6F30A4F5F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9792" windowHeight="5664" xr2:uid="{2DA1A733-42E6-40B7-8C76-4E54DEA7F056}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9792" windowHeight="5664" xr2:uid="{2DA1A733-42E6-40B7-8C76-4E54DEA7F056}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -886,7 +886,7 @@
   <dimension ref="B4:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>